<commit_message>
Entropy works, though with bottle-neck
</commit_message>
<xml_diff>
--- a/MonitoringTODOs.xlsx
+++ b/MonitoringTODOs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuval\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuval\Desktop\DistributedMonitoringOnceAgain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628D50D2-4E4B-47A1-870C-394A132CA98A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEB797B-B7B7-49FC-8815-577A02B23747}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{91B85CE4-EF0A-426E-BAF4-9725791231AC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Project</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Entropy Upper Bound &amp; Lower Bound - Unit Test</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>I presume it works fine due to previous work</t>
   </si>
   <si>
@@ -88,6 +85,21 @@
   </si>
   <si>
     <t>TODO</t>
+  </si>
+  <si>
+    <t>Entropy Bottle Neck</t>
+  </si>
+  <si>
+    <t>Binary search of INCREASE ENTROPY</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>PCA - Implement</t>
+  </si>
+  <si>
+    <t>todo</t>
   </si>
 </sst>
 </file>
@@ -385,20 +397,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,7 +728,7 @@
   <dimension ref="B1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,11 +740,11 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -751,7 +763,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>8</v>
@@ -762,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>3</v>
@@ -773,7 +785,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>3</v>
@@ -784,10 +796,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -795,7 +807,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>14</v>
@@ -806,10 +818,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -824,41 +836,53 @@
       </c>
     </row>
     <row r="12" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="19"/>
-      <c r="C12" s="20" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B13" s="5"/>
+      <c r="C13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="16"/>
+      <c r="C14" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="19"/>
-      <c r="C13" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="19"/>
-      <c r="C14" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="21" t="s">
+      <c r="C15" s="17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="18" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>

</xml_diff>